<commit_message>
Añadidos nuevos modelos y data set de train completo
</commit_message>
<xml_diff>
--- a/data/classification_J_33.xlsx
+++ b/data/classification_J_33.xlsx
@@ -556,7 +556,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -581,12 +581,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>+29</t>
+          <t>+28</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celta Vigo</t>
+          <t xml:space="preserve"> Rayo Vallecano</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1056,37 +1056,37 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>34</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>38</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>40</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Espanyol</t>
+          <t xml:space="preserve"> Celta Vigo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1126,17 +1126,17 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>37</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-8</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Elche</t>
+          <t xml:space="preserve"> Espanyol</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1171,22 +1171,22 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>37</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>39</t>
         </is>
       </c>
     </row>
@@ -1211,12 +1211,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rayo Vallecano</t>
+          <t xml:space="preserve"> Elche</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1236,22 +1236,22 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>36</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-8</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
           <t>38</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>-5</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>37</t>
         </is>
       </c>
     </row>

</xml_diff>